<commit_message>
commit dataserver config and task api
</commit_message>
<xml_diff>
--- a/Documents/Project Designs/Project Plan.xlsx
+++ b/Documents/Project Designs/Project Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="86">
   <si>
     <t>Done?</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>Prepare testing server</t>
+  </si>
+  <si>
+    <t>Write data test</t>
+  </si>
+  <si>
+    <t>Write data for testing</t>
   </si>
 </sst>
 </file>
@@ -870,7 +876,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -969,52 +975,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="11" fillId="5" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="5" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1025,75 +986,119 @@
     <xf numFmtId="164" fontId="3" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="8" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="5" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="5" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2863,50 +2868,50 @@
     </row>
     <row r="16" spans="2:28">
       <c r="B16" s="37"/>
-      <c r="C16" s="64">
+      <c r="C16" s="75">
         <v>41783</v>
       </c>
-      <c r="D16" s="63"/>
-      <c r="E16" s="62">
+      <c r="D16" s="76"/>
+      <c r="E16" s="77">
         <v>41794</v>
       </c>
-      <c r="F16" s="63"/>
-      <c r="G16" s="62">
+      <c r="F16" s="76"/>
+      <c r="G16" s="77">
         <v>41798</v>
       </c>
-      <c r="H16" s="63"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="62">
+      <c r="H16" s="76"/>
+      <c r="I16" s="77"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="77">
         <v>41812</v>
       </c>
-      <c r="L16" s="63"/>
-      <c r="M16" s="62">
+      <c r="L16" s="76"/>
+      <c r="M16" s="77">
         <v>41819</v>
       </c>
-      <c r="N16" s="63"/>
-      <c r="O16" s="63"/>
-      <c r="P16" s="63"/>
-      <c r="Q16" s="62">
+      <c r="N16" s="76"/>
+      <c r="O16" s="76"/>
+      <c r="P16" s="76"/>
+      <c r="Q16" s="77">
         <v>41826</v>
       </c>
-      <c r="R16" s="63"/>
-      <c r="S16" s="62">
+      <c r="R16" s="76"/>
+      <c r="S16" s="77">
         <v>41839</v>
       </c>
-      <c r="T16" s="63"/>
-      <c r="U16" s="62">
+      <c r="T16" s="76"/>
+      <c r="U16" s="77">
         <v>41845</v>
       </c>
-      <c r="V16" s="63"/>
-      <c r="W16" s="62">
+      <c r="V16" s="76"/>
+      <c r="W16" s="77">
         <v>41851</v>
       </c>
-      <c r="X16" s="63"/>
-      <c r="Y16" s="62">
+      <c r="X16" s="76"/>
+      <c r="Y16" s="77">
         <v>41852</v>
       </c>
-      <c r="Z16" s="63"/>
+      <c r="Z16" s="76"/>
       <c r="AA16" s="45"/>
       <c r="AB16" s="35"/>
     </row>
@@ -3231,11 +3236,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="S16:T16"/>
     <mergeCell ref="W16:X16"/>
     <mergeCell ref="Y16:Z16"/>
     <mergeCell ref="K16:L16"/>
@@ -3243,6 +3243,11 @@
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="Q16:R16"/>
     <mergeCell ref="U16:V16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="S16:T16"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3256,8 +3261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:H72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3321,20 +3326,20 @@
       <c r="B6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="85" t="s">
+      <c r="C6" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="85">
+      <c r="D6" s="67">
         <v>41770</v>
       </c>
-      <c r="E6" s="85" t="s">
+      <c r="E6" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="86" t="s">
+      <c r="F6" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
+      <c r="G6" s="98"/>
+      <c r="H6" s="98"/>
     </row>
     <row r="7" spans="2:8" ht="16.5" customHeight="1">
       <c r="B7" s="19" t="s">
@@ -3343,164 +3348,172 @@
       <c r="C7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="74">
+      <c r="D7" s="62">
         <v>41783</v>
       </c>
-      <c r="E7" s="74" t="s">
+      <c r="E7" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="75" t="s">
+      <c r="F7" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="76"/>
-      <c r="H7" s="77"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="101"/>
     </row>
     <row r="8" spans="2:8" ht="16.5" customHeight="1">
       <c r="B8" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="88" t="s">
+      <c r="C8" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="89">
+      <c r="D8" s="69">
         <v>41767</v>
       </c>
-      <c r="E8" s="85" t="s">
+      <c r="E8" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="90" t="s">
+      <c r="F8" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="91"/>
-      <c r="H8" s="92"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="83"/>
     </row>
     <row r="9" spans="2:8" ht="29.25" customHeight="1">
       <c r="B9" s="20"/>
       <c r="C9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="74">
+      <c r="D9" s="62">
         <v>41790</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="67" t="s">
+      <c r="F9" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="65"/>
-      <c r="H9" s="66"/>
+      <c r="G9" s="93"/>
+      <c r="H9" s="94"/>
     </row>
     <row r="10" spans="2:8" ht="27.75" customHeight="1">
       <c r="B10" s="20"/>
-      <c r="C10" s="88" t="s">
+      <c r="C10" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="89">
+      <c r="D10" s="69">
         <v>41790</v>
       </c>
-      <c r="E10" s="93" t="s">
+      <c r="E10" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="90" t="s">
+      <c r="F10" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="91"/>
-      <c r="H10" s="92"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="83"/>
     </row>
     <row r="11" spans="2:8" ht="27.75" customHeight="1">
       <c r="B11" s="20"/>
-      <c r="C11" s="79" t="s">
+      <c r="C11" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="80">
+      <c r="D11" s="65">
         <v>41790</v>
       </c>
-      <c r="E11" s="81" t="s">
+      <c r="E11" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="82" t="s">
+      <c r="F11" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="83"/>
-      <c r="H11" s="84"/>
+      <c r="G11" s="103"/>
+      <c r="H11" s="104"/>
     </row>
     <row r="12" spans="2:8" ht="30.75" customHeight="1">
       <c r="B12" s="20"/>
-      <c r="C12" s="88" t="s">
+      <c r="C12" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="89">
+      <c r="D12" s="69">
         <v>41794</v>
       </c>
-      <c r="E12" s="93" t="s">
+      <c r="E12" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="90" t="s">
+      <c r="F12" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="91"/>
-      <c r="H12" s="92"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="83"/>
     </row>
     <row r="13" spans="2:8" ht="16.5" customHeight="1">
       <c r="B13" s="20"/>
-      <c r="C13" s="79" t="s">
+      <c r="C13" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="80">
+      <c r="D13" s="65">
         <v>41798</v>
       </c>
-      <c r="E13" s="94" t="s">
+      <c r="E13" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="82" t="s">
+      <c r="F13" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="83"/>
-      <c r="H13" s="84"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="104"/>
     </row>
     <row r="14" spans="2:8" ht="29.25" customHeight="1">
       <c r="B14" s="20"/>
-      <c r="C14" s="88" t="s">
+      <c r="C14" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="89">
+      <c r="D14" s="69">
         <v>41804</v>
       </c>
-      <c r="E14" s="93" t="s">
+      <c r="E14" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="90" t="s">
+      <c r="F14" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="91"/>
-      <c r="H14" s="92"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="83"/>
     </row>
     <row r="15" spans="2:8" ht="16.5" customHeight="1">
       <c r="B15" s="20"/>
-      <c r="C15" s="79" t="s">
+      <c r="C15" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="80">
+      <c r="D15" s="65">
         <v>41805</v>
       </c>
-      <c r="E15" s="94" t="s">
+      <c r="E15" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="82" t="s">
+      <c r="F15" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="83"/>
-      <c r="H15" s="84"/>
+      <c r="G15" s="103"/>
+      <c r="H15" s="104"/>
     </row>
     <row r="16" spans="2:8" ht="16.5" customHeight="1">
       <c r="B16" s="20"/>
-      <c r="C16" s="95"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="97"/>
-      <c r="F16" s="98"/>
-      <c r="G16" s="99"/>
-      <c r="H16" s="100"/>
+      <c r="C16" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="65">
+        <v>41790</v>
+      </c>
+      <c r="E16" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="105" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="106"/>
+      <c r="H16" s="107"/>
     </row>
     <row r="17" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="18" spans="2:8" s="5" customFormat="1" ht="16.5" customHeight="1">
@@ -3533,28 +3546,28 @@
       <c r="E19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="71" t="s">
+      <c r="F19" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="72"/>
-      <c r="H19" s="73"/>
+      <c r="G19" s="95"/>
+      <c r="H19" s="96"/>
     </row>
     <row r="20" spans="2:8" ht="16.5" customHeight="1">
       <c r="B20" s="20"/>
-      <c r="C20" s="88" t="s">
+      <c r="C20" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="85">
+      <c r="D20" s="67">
         <v>41797</v>
       </c>
-      <c r="E20" s="85" t="s">
+      <c r="E20" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="90" t="s">
+      <c r="F20" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="91"/>
-      <c r="H20" s="92"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="83"/>
     </row>
     <row r="21" spans="2:8" ht="16.5" customHeight="1">
       <c r="B21" s="20"/>
@@ -3567,28 +3580,28 @@
       <c r="E21" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="67" t="s">
+      <c r="F21" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="65"/>
-      <c r="H21" s="66"/>
+      <c r="G21" s="93"/>
+      <c r="H21" s="94"/>
     </row>
     <row r="22" spans="2:8" ht="28.5" customHeight="1">
       <c r="B22" s="20"/>
-      <c r="C22" s="88" t="s">
+      <c r="C22" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="85">
+      <c r="D22" s="67">
         <v>41812</v>
       </c>
-      <c r="E22" s="93" t="s">
+      <c r="E22" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="90" t="s">
+      <c r="F22" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="91"/>
-      <c r="H22" s="92"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="83"/>
     </row>
     <row r="23" spans="2:8" ht="27" customHeight="1">
       <c r="B23" s="20"/>
@@ -3598,31 +3611,31 @@
       <c r="D23" s="12">
         <v>41819</v>
       </c>
-      <c r="E23" s="78" t="s">
+      <c r="E23" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="F23" s="67" t="s">
+      <c r="F23" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="65"/>
-      <c r="H23" s="66"/>
+      <c r="G23" s="93"/>
+      <c r="H23" s="94"/>
     </row>
     <row r="24" spans="2:8" ht="16.5" customHeight="1">
       <c r="B24" s="20"/>
-      <c r="C24" s="88" t="s">
+      <c r="C24" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="85">
+      <c r="D24" s="67">
         <v>41826</v>
       </c>
-      <c r="E24" s="85" t="s">
+      <c r="E24" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="90" t="s">
+      <c r="F24" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="G24" s="91"/>
-      <c r="H24" s="92"/>
+      <c r="G24" s="82"/>
+      <c r="H24" s="83"/>
     </row>
     <row r="25" spans="2:8" ht="38.25" customHeight="1">
       <c r="B25" s="20"/>
@@ -3632,32 +3645,32 @@
       <c r="D25" s="12">
         <v>41839</v>
       </c>
-      <c r="E25" s="78" t="s">
+      <c r="E25" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="67" t="s">
+      <c r="F25" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="G25" s="65"/>
-      <c r="H25" s="66"/>
+      <c r="G25" s="93"/>
+      <c r="H25" s="94"/>
     </row>
     <row r="26" spans="2:8" ht="16.5" customHeight="1">
       <c r="B26" s="20"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="85"/>
-      <c r="E26" s="85"/>
-      <c r="F26" s="90"/>
-      <c r="G26" s="91"/>
-      <c r="H26" s="92"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="81"/>
+      <c r="G26" s="82"/>
+      <c r="H26" s="83"/>
     </row>
     <row r="27" spans="2:8" ht="16.5" customHeight="1">
       <c r="B27" s="20"/>
       <c r="C27" s="13"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="70"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="85"/>
+      <c r="H27" s="86"/>
     </row>
     <row r="28" spans="2:8" ht="16.5" customHeight="1">
       <c r="B28" s="7"/>
@@ -3675,11 +3688,11 @@
       <c r="E29" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="101" t="s">
+      <c r="F29" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="102"/>
-      <c r="H29" s="103"/>
+      <c r="G29" s="88"/>
+      <c r="H29" s="89"/>
     </row>
     <row r="30" spans="2:8" ht="16.5" customHeight="1">
       <c r="B30" s="19"/>
@@ -3692,30 +3705,30 @@
       <c r="E30" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="71" t="s">
+      <c r="F30" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="72"/>
-      <c r="H30" s="73"/>
+      <c r="G30" s="95"/>
+      <c r="H30" s="96"/>
     </row>
     <row r="31" spans="2:8" ht="16.5" customHeight="1">
       <c r="B31" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="88" t="s">
+      <c r="C31" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="85">
+      <c r="D31" s="67">
         <v>41814</v>
       </c>
-      <c r="E31" s="85" t="s">
+      <c r="E31" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="90" t="s">
+      <c r="F31" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="G31" s="91"/>
-      <c r="H31" s="92"/>
+      <c r="G31" s="82"/>
+      <c r="H31" s="83"/>
     </row>
     <row r="32" spans="2:8" ht="16.5" customHeight="1">
       <c r="B32" s="20"/>
@@ -3728,28 +3741,28 @@
       <c r="E32" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F32" s="67" t="s">
+      <c r="F32" s="78" t="s">
         <v>52</v>
       </c>
-      <c r="G32" s="65"/>
-      <c r="H32" s="66"/>
+      <c r="G32" s="93"/>
+      <c r="H32" s="94"/>
     </row>
     <row r="33" spans="2:8" ht="39" customHeight="1">
       <c r="B33" s="20"/>
-      <c r="C33" s="88" t="s">
+      <c r="C33" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="85">
+      <c r="D33" s="67">
         <v>41812</v>
       </c>
-      <c r="E33" s="93" t="s">
+      <c r="E33" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="F33" s="90" t="s">
+      <c r="F33" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="G33" s="91"/>
-      <c r="H33" s="92"/>
+      <c r="G33" s="82"/>
+      <c r="H33" s="83"/>
     </row>
     <row r="34" spans="2:8" ht="36" customHeight="1">
       <c r="B34" s="20"/>
@@ -3759,31 +3772,31 @@
       <c r="D34" s="16">
         <v>41812</v>
       </c>
-      <c r="E34" s="104" t="s">
+      <c r="E34" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="F34" s="67" t="s">
+      <c r="F34" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="G34" s="65"/>
-      <c r="H34" s="66"/>
+      <c r="G34" s="93"/>
+      <c r="H34" s="94"/>
     </row>
     <row r="35" spans="2:8" ht="16.5" customHeight="1">
       <c r="B35" s="20"/>
-      <c r="C35" s="88" t="s">
+      <c r="C35" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="85">
+      <c r="D35" s="67">
         <v>41819</v>
       </c>
-      <c r="E35" s="85" t="s">
+      <c r="E35" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="F35" s="90" t="s">
+      <c r="F35" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="G35" s="91"/>
-      <c r="H35" s="92"/>
+      <c r="G35" s="82"/>
+      <c r="H35" s="83"/>
     </row>
     <row r="36" spans="2:8" ht="27.75" customHeight="1">
       <c r="B36" s="20"/>
@@ -3796,29 +3809,29 @@
       <c r="E36" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F36" s="67" t="s">
+      <c r="F36" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="65"/>
-      <c r="H36" s="66"/>
+      <c r="G36" s="93"/>
+      <c r="H36" s="94"/>
     </row>
     <row r="37" spans="2:8" ht="16.5" customHeight="1">
       <c r="B37" s="20"/>
-      <c r="C37" s="88"/>
-      <c r="D37" s="85"/>
-      <c r="E37" s="85"/>
-      <c r="F37" s="90"/>
-      <c r="G37" s="91"/>
-      <c r="H37" s="92"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="81"/>
+      <c r="G37" s="82"/>
+      <c r="H37" s="83"/>
     </row>
     <row r="38" spans="2:8" ht="16.5" customHeight="1">
       <c r="B38" s="20"/>
       <c r="C38" s="17"/>
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="69"/>
-      <c r="H38" s="70"/>
+      <c r="F38" s="84"/>
+      <c r="G38" s="85"/>
+      <c r="H38" s="86"/>
     </row>
     <row r="41" spans="2:8">
       <c r="B41" s="6" t="s">
@@ -3833,11 +3846,11 @@
       <c r="E41" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F41" s="101" t="s">
+      <c r="F41" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="G41" s="102"/>
-      <c r="H41" s="103"/>
+      <c r="G41" s="88"/>
+      <c r="H41" s="89"/>
     </row>
     <row r="42" spans="2:8" ht="14.25">
       <c r="B42" s="19"/>
@@ -3850,28 +3863,28 @@
       <c r="E42" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F42" s="71" t="s">
+      <c r="F42" s="90" t="s">
         <v>61</v>
       </c>
-      <c r="G42" s="107"/>
-      <c r="H42" s="108"/>
+      <c r="G42" s="91"/>
+      <c r="H42" s="92"/>
     </row>
     <row r="43" spans="2:8" ht="14.25" customHeight="1">
       <c r="B43" s="20"/>
-      <c r="C43" s="88" t="s">
+      <c r="C43" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D43" s="85">
+      <c r="D43" s="67">
         <v>41814</v>
       </c>
-      <c r="E43" s="85" t="s">
+      <c r="E43" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="F43" s="90" t="s">
+      <c r="F43" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="G43" s="91"/>
-      <c r="H43" s="92"/>
+      <c r="G43" s="82"/>
+      <c r="H43" s="83"/>
     </row>
     <row r="44" spans="2:8" ht="25.5">
       <c r="B44" s="20"/>
@@ -3881,31 +3894,31 @@
       <c r="D44" s="16">
         <v>41798</v>
       </c>
-      <c r="E44" s="94" t="s">
+      <c r="E44" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="F44" s="67" t="s">
+      <c r="F44" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="G44" s="105"/>
-      <c r="H44" s="106"/>
+      <c r="G44" s="79"/>
+      <c r="H44" s="80"/>
     </row>
     <row r="45" spans="2:8" ht="25.5">
       <c r="B45" s="20"/>
-      <c r="C45" s="88" t="s">
+      <c r="C45" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="85">
+      <c r="D45" s="67">
         <v>41812</v>
       </c>
-      <c r="E45" s="85" t="s">
+      <c r="E45" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="F45" s="90" t="s">
+      <c r="F45" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="G45" s="91"/>
-      <c r="H45" s="92"/>
+      <c r="G45" s="82"/>
+      <c r="H45" s="83"/>
     </row>
     <row r="46" spans="2:8" ht="25.5">
       <c r="B46" s="20"/>
@@ -3915,50 +3928,50 @@
       <c r="D46" s="16">
         <v>41812</v>
       </c>
-      <c r="E46" s="94" t="s">
+      <c r="E46" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="F46" s="67" t="s">
+      <c r="F46" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="G46" s="105"/>
-      <c r="H46" s="106"/>
+      <c r="G46" s="79"/>
+      <c r="H46" s="80"/>
     </row>
     <row r="47" spans="2:8" ht="14.25">
       <c r="B47" s="20"/>
-      <c r="C47" s="88"/>
-      <c r="D47" s="85"/>
-      <c r="E47" s="85"/>
-      <c r="F47" s="90"/>
-      <c r="G47" s="91"/>
-      <c r="H47" s="92"/>
+      <c r="C47" s="68"/>
+      <c r="D47" s="67"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="81"/>
+      <c r="G47" s="82"/>
+      <c r="H47" s="83"/>
     </row>
     <row r="48" spans="2:8" ht="14.25">
       <c r="B48" s="20"/>
       <c r="C48" s="21"/>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
-      <c r="F48" s="67"/>
-      <c r="G48" s="105"/>
-      <c r="H48" s="106"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="79"/>
+      <c r="H48" s="80"/>
     </row>
     <row r="49" spans="2:8" ht="14.25">
       <c r="B49" s="20"/>
-      <c r="C49" s="88"/>
-      <c r="D49" s="85"/>
-      <c r="E49" s="85"/>
-      <c r="F49" s="90"/>
-      <c r="G49" s="91"/>
-      <c r="H49" s="92"/>
+      <c r="C49" s="68"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="67"/>
+      <c r="F49" s="81"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="83"/>
     </row>
     <row r="50" spans="2:8" ht="14.25">
       <c r="B50" s="20"/>
       <c r="C50" s="22"/>
       <c r="D50" s="18"/>
       <c r="E50" s="18"/>
-      <c r="F50" s="68"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="70"/>
+      <c r="F50" s="84"/>
+      <c r="G50" s="85"/>
+      <c r="H50" s="86"/>
     </row>
     <row r="52" spans="2:8">
       <c r="B52" s="6" t="s">
@@ -3973,11 +3986,11 @@
       <c r="E52" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F52" s="101" t="s">
+      <c r="F52" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="G52" s="102"/>
-      <c r="H52" s="103"/>
+      <c r="G52" s="88"/>
+      <c r="H52" s="89"/>
     </row>
     <row r="53" spans="2:8" ht="14.25">
       <c r="B53" s="19"/>
@@ -3990,28 +4003,28 @@
       <c r="E53" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F53" s="71" t="s">
+      <c r="F53" s="90" t="s">
         <v>61</v>
       </c>
-      <c r="G53" s="107"/>
-      <c r="H53" s="108"/>
+      <c r="G53" s="91"/>
+      <c r="H53" s="92"/>
     </row>
     <row r="54" spans="2:8" ht="14.25">
       <c r="B54" s="20"/>
-      <c r="C54" s="88" t="s">
+      <c r="C54" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D54" s="85">
+      <c r="D54" s="67">
         <v>41784</v>
       </c>
-      <c r="E54" s="85" t="s">
+      <c r="E54" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="F54" s="90" t="s">
+      <c r="F54" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="G54" s="91"/>
-      <c r="H54" s="92"/>
+      <c r="G54" s="82"/>
+      <c r="H54" s="83"/>
     </row>
     <row r="55" spans="2:8" ht="25.5">
       <c r="B55" s="20"/>
@@ -4021,29 +4034,29 @@
       <c r="D55" s="16">
         <v>41786</v>
       </c>
-      <c r="E55" s="94" t="s">
+      <c r="E55" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="F55" s="67"/>
-      <c r="G55" s="105"/>
-      <c r="H55" s="106"/>
+      <c r="F55" s="78"/>
+      <c r="G55" s="79"/>
+      <c r="H55" s="80"/>
     </row>
     <row r="56" spans="2:8" ht="25.5">
       <c r="B56" s="20"/>
-      <c r="C56" s="88" t="s">
+      <c r="C56" s="68" t="s">
         <v>72</v>
       </c>
-      <c r="D56" s="85">
+      <c r="D56" s="67">
         <v>41791</v>
       </c>
-      <c r="E56" s="85" t="s">
+      <c r="E56" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="F56" s="90" t="s">
+      <c r="F56" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="G56" s="91"/>
-      <c r="H56" s="92"/>
+      <c r="G56" s="82"/>
+      <c r="H56" s="83"/>
     </row>
     <row r="57" spans="2:8" ht="38.25">
       <c r="B57" s="20"/>
@@ -4053,31 +4066,31 @@
       <c r="D57" s="16">
         <v>41805</v>
       </c>
-      <c r="E57" s="81" t="s">
+      <c r="E57" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="F57" s="67" t="s">
+      <c r="F57" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="G57" s="105"/>
-      <c r="H57" s="106"/>
+      <c r="G57" s="79"/>
+      <c r="H57" s="80"/>
     </row>
     <row r="58" spans="2:8" ht="38.25">
       <c r="B58" s="20"/>
-      <c r="C58" s="88" t="s">
+      <c r="C58" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="D58" s="85">
+      <c r="D58" s="67">
         <v>41812</v>
       </c>
-      <c r="E58" s="93" t="s">
+      <c r="E58" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="F58" s="90" t="s">
+      <c r="F58" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="G58" s="91"/>
-      <c r="H58" s="92"/>
+      <c r="G58" s="82"/>
+      <c r="H58" s="83"/>
     </row>
     <row r="59" spans="2:8" ht="25.5">
       <c r="B59" s="20"/>
@@ -4087,32 +4100,32 @@
       <c r="D59" s="16">
         <v>41812</v>
       </c>
-      <c r="E59" s="104" t="s">
+      <c r="E59" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="F59" s="67" t="s">
+      <c r="F59" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="G59" s="105"/>
-      <c r="H59" s="106"/>
+      <c r="G59" s="79"/>
+      <c r="H59" s="80"/>
     </row>
     <row r="60" spans="2:8" ht="14.25">
       <c r="B60" s="20"/>
-      <c r="C60" s="88"/>
-      <c r="D60" s="85"/>
-      <c r="E60" s="85"/>
-      <c r="F60" s="90"/>
-      <c r="G60" s="91"/>
-      <c r="H60" s="92"/>
+      <c r="C60" s="68"/>
+      <c r="D60" s="67"/>
+      <c r="E60" s="67"/>
+      <c r="F60" s="81"/>
+      <c r="G60" s="82"/>
+      <c r="H60" s="83"/>
     </row>
     <row r="61" spans="2:8" ht="14.25">
       <c r="B61" s="20"/>
       <c r="C61" s="22"/>
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
-      <c r="F61" s="68"/>
-      <c r="G61" s="69"/>
-      <c r="H61" s="70"/>
+      <c r="F61" s="84"/>
+      <c r="G61" s="85"/>
+      <c r="H61" s="86"/>
     </row>
     <row r="63" spans="2:8">
       <c r="B63" s="6" t="s">
@@ -4127,11 +4140,11 @@
       <c r="E63" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F63" s="101" t="s">
+      <c r="F63" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="G63" s="102"/>
-      <c r="H63" s="103"/>
+      <c r="G63" s="88"/>
+      <c r="H63" s="89"/>
     </row>
     <row r="64" spans="2:8" ht="38.25">
       <c r="B64" s="19"/>
@@ -4144,140 +4157,93 @@
       <c r="E64" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F64" s="71" t="s">
+      <c r="F64" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="G64" s="107"/>
-      <c r="H64" s="108"/>
+      <c r="G64" s="91"/>
+      <c r="H64" s="92"/>
     </row>
     <row r="65" spans="2:8" ht="25.5">
       <c r="B65" s="20"/>
-      <c r="C65" s="88" t="s">
+      <c r="C65" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="D65" s="85">
+      <c r="D65" s="67">
         <v>41802</v>
       </c>
-      <c r="E65" s="85" t="s">
+      <c r="E65" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="F65" s="90"/>
-      <c r="G65" s="91"/>
-      <c r="H65" s="92"/>
+      <c r="F65" s="81"/>
+      <c r="G65" s="82"/>
+      <c r="H65" s="83"/>
     </row>
     <row r="66" spans="2:8" ht="14.25">
       <c r="B66" s="20"/>
       <c r="C66" s="21"/>
       <c r="D66" s="16"/>
-      <c r="E66" s="94"/>
-      <c r="F66" s="67"/>
-      <c r="G66" s="105"/>
-      <c r="H66" s="106"/>
+      <c r="E66" s="71"/>
+      <c r="F66" s="78"/>
+      <c r="G66" s="79"/>
+      <c r="H66" s="80"/>
     </row>
     <row r="67" spans="2:8" ht="14.25">
       <c r="B67" s="20"/>
-      <c r="C67" s="88"/>
-      <c r="D67" s="85"/>
-      <c r="E67" s="85"/>
-      <c r="F67" s="90"/>
-      <c r="G67" s="91"/>
-      <c r="H67" s="92"/>
+      <c r="C67" s="68"/>
+      <c r="D67" s="67"/>
+      <c r="E67" s="67"/>
+      <c r="F67" s="81"/>
+      <c r="G67" s="82"/>
+      <c r="H67" s="83"/>
     </row>
     <row r="68" spans="2:8" ht="14.25">
       <c r="B68" s="20"/>
       <c r="C68" s="21"/>
       <c r="D68" s="16"/>
-      <c r="E68" s="81"/>
-      <c r="F68" s="67"/>
-      <c r="G68" s="105"/>
-      <c r="H68" s="106"/>
+      <c r="E68" s="66"/>
+      <c r="F68" s="78"/>
+      <c r="G68" s="79"/>
+      <c r="H68" s="80"/>
     </row>
     <row r="69" spans="2:8" ht="14.25">
       <c r="B69" s="20"/>
-      <c r="C69" s="88"/>
-      <c r="D69" s="85"/>
-      <c r="E69" s="93"/>
-      <c r="F69" s="90"/>
-      <c r="G69" s="91"/>
-      <c r="H69" s="92"/>
+      <c r="C69" s="68"/>
+      <c r="D69" s="67"/>
+      <c r="E69" s="70"/>
+      <c r="F69" s="81"/>
+      <c r="G69" s="82"/>
+      <c r="H69" s="83"/>
     </row>
     <row r="70" spans="2:8" ht="14.25">
       <c r="B70" s="20"/>
       <c r="C70" s="21"/>
       <c r="D70" s="16"/>
-      <c r="E70" s="104"/>
-      <c r="F70" s="67"/>
-      <c r="G70" s="105"/>
-      <c r="H70" s="106"/>
+      <c r="E70" s="74"/>
+      <c r="F70" s="78"/>
+      <c r="G70" s="79"/>
+      <c r="H70" s="80"/>
     </row>
     <row r="71" spans="2:8" ht="14.25">
       <c r="B71" s="20"/>
-      <c r="C71" s="88"/>
-      <c r="D71" s="85"/>
-      <c r="E71" s="85"/>
-      <c r="F71" s="90"/>
-      <c r="G71" s="91"/>
-      <c r="H71" s="92"/>
+      <c r="C71" s="68"/>
+      <c r="D71" s="67"/>
+      <c r="E71" s="67"/>
+      <c r="F71" s="81"/>
+      <c r="G71" s="82"/>
+      <c r="H71" s="83"/>
     </row>
     <row r="72" spans="2:8" ht="14.25">
       <c r="B72" s="20"/>
       <c r="C72" s="22"/>
       <c r="D72" s="18"/>
       <c r="E72" s="18"/>
-      <c r="F72" s="68"/>
-      <c r="G72" s="69"/>
-      <c r="H72" s="70"/>
+      <c r="F72" s="84"/>
+      <c r="G72" s="85"/>
+      <c r="H72" s="86"/>
     </row>
   </sheetData>
   <autoFilter ref="B5:B38"/>
   <mergeCells count="60">
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F29:H29"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="F8:H8"/>
@@ -4291,6 +4257,53 @@
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F72:H72"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
commit code for task-api, lang-api, profile-api
</commit_message>
<xml_diff>
--- a/Documents/Project Designs/Project Plan.xlsx
+++ b/Documents/Project Designs/Project Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="85">
   <si>
     <t>Done?</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Lang/PBL module</t>
-  </si>
-  <si>
-    <t>Phương T</t>
   </si>
   <si>
     <t>Anh Đ</t>
@@ -1002,103 +999,103 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="11" fillId="5" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="16" fontId="11" fillId="5" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="5" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2868,47 +2865,47 @@
     </row>
     <row r="16" spans="2:28">
       <c r="B16" s="37"/>
-      <c r="C16" s="75">
+      <c r="C16" s="77">
         <v>41783</v>
       </c>
       <c r="D16" s="76"/>
-      <c r="E16" s="77">
+      <c r="E16" s="75">
         <v>41794</v>
       </c>
       <c r="F16" s="76"/>
-      <c r="G16" s="77">
+      <c r="G16" s="75">
         <v>41798</v>
       </c>
       <c r="H16" s="76"/>
-      <c r="I16" s="77"/>
+      <c r="I16" s="75"/>
       <c r="J16" s="76"/>
-      <c r="K16" s="77">
+      <c r="K16" s="75">
         <v>41812</v>
       </c>
       <c r="L16" s="76"/>
-      <c r="M16" s="77">
+      <c r="M16" s="75">
         <v>41819</v>
       </c>
       <c r="N16" s="76"/>
       <c r="O16" s="76"/>
       <c r="P16" s="76"/>
-      <c r="Q16" s="77">
+      <c r="Q16" s="75">
         <v>41826</v>
       </c>
       <c r="R16" s="76"/>
-      <c r="S16" s="77">
+      <c r="S16" s="75">
         <v>41839</v>
       </c>
       <c r="T16" s="76"/>
-      <c r="U16" s="77">
+      <c r="U16" s="75">
         <v>41845</v>
       </c>
       <c r="V16" s="76"/>
-      <c r="W16" s="77">
+      <c r="W16" s="75">
         <v>41851</v>
       </c>
       <c r="X16" s="76"/>
-      <c r="Y16" s="77">
+      <c r="Y16" s="75">
         <v>41852</v>
       </c>
       <c r="Z16" s="76"/>
@@ -3236,6 +3233,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="S16:T16"/>
     <mergeCell ref="W16:X16"/>
     <mergeCell ref="Y16:Z16"/>
     <mergeCell ref="K16:L16"/>
@@ -3243,11 +3245,6 @@
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="Q16:R16"/>
     <mergeCell ref="U16:V16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="S16:T16"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3261,8 +3258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:H72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3281,7 +3278,7 @@
   <sheetData>
     <row r="1" spans="2:8" ht="41.25" customHeight="1">
       <c r="B1" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
@@ -3308,7 +3305,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>7</v>
@@ -3324,7 +3321,7 @@
     </row>
     <row r="6" spans="2:8" ht="16.5" customHeight="1">
       <c r="B6" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="67" t="s">
         <v>2</v>
@@ -3335,15 +3332,15 @@
       <c r="E6" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="97" t="s">
+      <c r="F6" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
     </row>
     <row r="7" spans="2:8" ht="16.5" customHeight="1">
       <c r="B7" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>13</v>
@@ -3354,15 +3351,15 @@
       <c r="E7" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="99" t="s">
+      <c r="F7" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="100"/>
-      <c r="H7" s="101"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="88"/>
     </row>
     <row r="8" spans="2:8" ht="16.5" customHeight="1">
       <c r="B8" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="68" t="s">
         <v>10</v>
@@ -3373,11 +3370,11 @@
       <c r="E8" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="81" t="s">
+      <c r="F8" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="82"/>
-      <c r="H8" s="83"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="80"/>
     </row>
     <row r="9" spans="2:8" ht="29.25" customHeight="1">
       <c r="B9" s="20"/>
@@ -3387,36 +3384,38 @@
       <c r="D9" s="62">
         <v>41790</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="78" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="93"/>
-      <c r="H9" s="94"/>
+      <c r="E9" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="83" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="84"/>
+      <c r="H9" s="85"/>
     </row>
     <row r="10" spans="2:8" ht="27.75" customHeight="1">
       <c r="B10" s="20"/>
       <c r="C10" s="68" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="69">
         <v>41790</v>
       </c>
       <c r="E10" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="79"/>
+      <c r="H10" s="80"/>
+    </row>
+    <row r="11" spans="2:8" ht="27.75" customHeight="1">
+      <c r="B11" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="81" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="82"/>
-      <c r="H10" s="83"/>
-    </row>
-    <row r="11" spans="2:8" ht="27.75" customHeight="1">
-      <c r="B11" s="20"/>
       <c r="C11" s="64" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="65">
         <v>41790</v>
@@ -3424,67 +3423,67 @@
       <c r="E11" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="102" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="103"/>
-      <c r="H11" s="104"/>
+      <c r="F11" s="89" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="90"/>
+      <c r="H11" s="91"/>
     </row>
     <row r="12" spans="2:8" ht="30.75" customHeight="1">
       <c r="B12" s="20"/>
       <c r="C12" s="68" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="69">
         <v>41794</v>
       </c>
       <c r="E12" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="81" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="82"/>
-      <c r="H12" s="83"/>
+        <v>19</v>
+      </c>
+      <c r="F12" s="78" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="79"/>
+      <c r="H12" s="80"/>
     </row>
     <row r="13" spans="2:8" ht="16.5" customHeight="1">
       <c r="B13" s="20"/>
       <c r="C13" s="64" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="65">
         <v>41798</v>
       </c>
       <c r="E13" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="102" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="103"/>
-      <c r="H13" s="104"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="91"/>
     </row>
     <row r="14" spans="2:8" ht="29.25" customHeight="1">
       <c r="B14" s="20"/>
       <c r="C14" s="68" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="69">
         <v>41804</v>
       </c>
       <c r="E14" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="81" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="82"/>
-      <c r="H14" s="83"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="80"/>
     </row>
     <row r="15" spans="2:8" ht="16.5" customHeight="1">
       <c r="B15" s="20"/>
       <c r="C15" s="64" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="65">
         <v>41805</v>
@@ -3492,16 +3491,18 @@
       <c r="E15" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="102" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="103"/>
-      <c r="H15" s="104"/>
+      <c r="F15" s="89" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="90"/>
+      <c r="H15" s="91"/>
     </row>
     <row r="16" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B16" s="20"/>
+      <c r="B16" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="C16" s="73" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D16" s="65">
         <v>41790</v>
@@ -3509,11 +3510,11 @@
       <c r="E16" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="105" t="s">
-        <v>85</v>
-      </c>
-      <c r="G16" s="106"/>
-      <c r="H16" s="107"/>
+      <c r="F16" s="92" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="93"/>
+      <c r="H16" s="94"/>
     </row>
     <row r="17" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="18" spans="2:8" s="5" customFormat="1" ht="16.5" customHeight="1">
@@ -3521,7 +3522,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>7</v>
@@ -3546,11 +3547,11 @@
       <c r="E19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="90" t="s">
+      <c r="F19" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="95"/>
-      <c r="H19" s="96"/>
+      <c r="G19" s="96"/>
+      <c r="H19" s="97"/>
     </row>
     <row r="20" spans="2:8" ht="16.5" customHeight="1">
       <c r="B20" s="20"/>
@@ -3561,116 +3562,116 @@
         <v>41797</v>
       </c>
       <c r="E20" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="81" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="82"/>
-      <c r="H20" s="83"/>
+        <v>16</v>
+      </c>
+      <c r="F20" s="78" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="79"/>
+      <c r="H20" s="80"/>
     </row>
     <row r="21" spans="2:8" ht="16.5" customHeight="1">
       <c r="B21" s="20"/>
       <c r="C21" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="12">
         <v>41812</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="78" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="93"/>
-      <c r="H21" s="94"/>
+        <v>16</v>
+      </c>
+      <c r="F21" s="83" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="84"/>
+      <c r="H21" s="85"/>
     </row>
     <row r="22" spans="2:8" ht="28.5" customHeight="1">
       <c r="B22" s="20"/>
       <c r="C22" s="68" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" s="67">
         <v>41812</v>
       </c>
       <c r="E22" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="82"/>
-      <c r="H22" s="83"/>
+      <c r="F22" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="79"/>
+      <c r="H22" s="80"/>
     </row>
     <row r="23" spans="2:8" ht="27" customHeight="1">
       <c r="B23" s="20"/>
       <c r="C23" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="12">
         <v>41819</v>
       </c>
       <c r="E23" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="F23" s="78" t="s">
-        <v>44</v>
-      </c>
-      <c r="G23" s="93"/>
-      <c r="H23" s="94"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="85"/>
     </row>
     <row r="24" spans="2:8" ht="16.5" customHeight="1">
       <c r="B24" s="20"/>
       <c r="C24" s="68" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" s="67">
         <v>41826</v>
       </c>
       <c r="E24" s="67" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="81" t="s">
-        <v>45</v>
-      </c>
-      <c r="G24" s="82"/>
-      <c r="H24" s="83"/>
+        <v>23</v>
+      </c>
+      <c r="F24" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="79"/>
+      <c r="H24" s="80"/>
     </row>
     <row r="25" spans="2:8" ht="38.25" customHeight="1">
       <c r="B25" s="20"/>
       <c r="C25" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" s="12">
         <v>41839</v>
       </c>
       <c r="E25" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="78" t="s">
-        <v>47</v>
-      </c>
-      <c r="G25" s="93"/>
-      <c r="H25" s="94"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="85"/>
     </row>
     <row r="26" spans="2:8" ht="16.5" customHeight="1">
       <c r="B26" s="20"/>
       <c r="C26" s="68"/>
       <c r="D26" s="67"/>
       <c r="E26" s="67"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="82"/>
-      <c r="H26" s="83"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="80"/>
     </row>
     <row r="27" spans="2:8" ht="16.5" customHeight="1">
       <c r="B27" s="20"/>
       <c r="C27" s="13"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="85"/>
-      <c r="H27" s="86"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="99"/>
+      <c r="H27" s="100"/>
     </row>
     <row r="28" spans="2:8" ht="16.5" customHeight="1">
       <c r="B28" s="7"/>
@@ -3680,7 +3681,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="26" t="s">
         <v>7</v>
@@ -3688,11 +3689,11 @@
       <c r="E29" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="87" t="s">
+      <c r="F29" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="88"/>
-      <c r="H29" s="89"/>
+      <c r="G29" s="102"/>
+      <c r="H29" s="103"/>
     </row>
     <row r="30" spans="2:8" ht="16.5" customHeight="1">
       <c r="B30" s="19"/>
@@ -3705,15 +3706,15 @@
       <c r="E30" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="90" t="s">
+      <c r="F30" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="95"/>
-      <c r="H30" s="96"/>
+      <c r="G30" s="96"/>
+      <c r="H30" s="97"/>
     </row>
     <row r="31" spans="2:8" ht="16.5" customHeight="1">
       <c r="B31" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31" s="68" t="s">
         <v>1</v>
@@ -3722,123 +3723,123 @@
         <v>41814</v>
       </c>
       <c r="E31" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="F31" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="81" t="s">
-        <v>50</v>
-      </c>
-      <c r="G31" s="82"/>
-      <c r="H31" s="83"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="80"/>
     </row>
     <row r="32" spans="2:8" ht="16.5" customHeight="1">
       <c r="B32" s="20"/>
       <c r="C32" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D32" s="16">
         <v>41798</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F32" s="78" t="s">
-        <v>52</v>
-      </c>
-      <c r="G32" s="93"/>
-      <c r="H32" s="94"/>
+        <v>48</v>
+      </c>
+      <c r="F32" s="83" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" s="84"/>
+      <c r="H32" s="85"/>
     </row>
     <row r="33" spans="2:8" ht="39" customHeight="1">
       <c r="B33" s="20"/>
       <c r="C33" s="68" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D33" s="67">
         <v>41812</v>
       </c>
       <c r="E33" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="81" t="s">
-        <v>54</v>
-      </c>
-      <c r="G33" s="82"/>
-      <c r="H33" s="83"/>
+        <v>55</v>
+      </c>
+      <c r="F33" s="78" t="s">
+        <v>53</v>
+      </c>
+      <c r="G33" s="79"/>
+      <c r="H33" s="80"/>
     </row>
     <row r="34" spans="2:8" ht="36" customHeight="1">
       <c r="B34" s="20"/>
       <c r="C34" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D34" s="16">
         <v>41812</v>
       </c>
       <c r="E34" s="74" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="F34" s="78" t="s">
-        <v>57</v>
-      </c>
-      <c r="G34" s="93"/>
-      <c r="H34" s="94"/>
+      <c r="G34" s="84"/>
+      <c r="H34" s="85"/>
     </row>
     <row r="35" spans="2:8" ht="16.5" customHeight="1">
       <c r="B35" s="20"/>
       <c r="C35" s="68" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D35" s="67">
         <v>41819</v>
       </c>
       <c r="E35" s="67" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35" s="81" t="s">
-        <v>58</v>
-      </c>
-      <c r="G35" s="82"/>
-      <c r="H35" s="83"/>
+        <v>23</v>
+      </c>
+      <c r="F35" s="78" t="s">
+        <v>57</v>
+      </c>
+      <c r="G35" s="79"/>
+      <c r="H35" s="80"/>
     </row>
     <row r="36" spans="2:8" ht="27.75" customHeight="1">
       <c r="B36" s="20"/>
       <c r="C36" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D36" s="16">
         <v>41826</v>
       </c>
       <c r="E36" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="F36" s="78" t="s">
-        <v>60</v>
-      </c>
-      <c r="G36" s="93"/>
-      <c r="H36" s="94"/>
+      <c r="G36" s="84"/>
+      <c r="H36" s="85"/>
     </row>
     <row r="37" spans="2:8" ht="16.5" customHeight="1">
       <c r="B37" s="20"/>
       <c r="C37" s="68"/>
       <c r="D37" s="67"/>
       <c r="E37" s="67"/>
-      <c r="F37" s="81"/>
-      <c r="G37" s="82"/>
-      <c r="H37" s="83"/>
+      <c r="F37" s="78"/>
+      <c r="G37" s="79"/>
+      <c r="H37" s="80"/>
     </row>
     <row r="38" spans="2:8" ht="16.5" customHeight="1">
       <c r="B38" s="20"/>
       <c r="C38" s="17"/>
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
-      <c r="F38" s="84"/>
-      <c r="G38" s="85"/>
-      <c r="H38" s="86"/>
+      <c r="F38" s="98"/>
+      <c r="G38" s="99"/>
+      <c r="H38" s="100"/>
     </row>
     <row r="41" spans="2:8">
       <c r="B41" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D41" s="26" t="s">
         <v>7</v>
@@ -3846,11 +3847,11 @@
       <c r="E41" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F41" s="87" t="s">
+      <c r="F41" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="G41" s="88"/>
-      <c r="H41" s="89"/>
+      <c r="G41" s="102"/>
+      <c r="H41" s="103"/>
     </row>
     <row r="42" spans="2:8" ht="14.25">
       <c r="B42" s="19"/>
@@ -3863,11 +3864,11 @@
       <c r="E42" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F42" s="90" t="s">
-        <v>61</v>
-      </c>
-      <c r="G42" s="91"/>
-      <c r="H42" s="92"/>
+      <c r="F42" s="95" t="s">
+        <v>60</v>
+      </c>
+      <c r="G42" s="104"/>
+      <c r="H42" s="105"/>
     </row>
     <row r="43" spans="2:8" ht="14.25" customHeight="1">
       <c r="B43" s="20"/>
@@ -3878,107 +3879,107 @@
         <v>41814</v>
       </c>
       <c r="E43" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="F43" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="F43" s="81" t="s">
-        <v>63</v>
-      </c>
-      <c r="G43" s="82"/>
-      <c r="H43" s="83"/>
+      <c r="G43" s="79"/>
+      <c r="H43" s="80"/>
     </row>
     <row r="44" spans="2:8" ht="25.5">
       <c r="B44" s="20"/>
       <c r="C44" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D44" s="16">
         <v>41798</v>
       </c>
       <c r="E44" s="71" t="s">
-        <v>62</v>
-      </c>
-      <c r="F44" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="G44" s="79"/>
-      <c r="H44" s="80"/>
+        <v>61</v>
+      </c>
+      <c r="F44" s="83" t="s">
+        <v>63</v>
+      </c>
+      <c r="G44" s="106"/>
+      <c r="H44" s="107"/>
     </row>
     <row r="45" spans="2:8" ht="25.5">
       <c r="B45" s="20"/>
       <c r="C45" s="68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D45" s="67">
         <v>41812</v>
       </c>
       <c r="E45" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="F45" s="81" t="s">
-        <v>64</v>
-      </c>
-      <c r="G45" s="82"/>
-      <c r="H45" s="83"/>
+        <v>61</v>
+      </c>
+      <c r="F45" s="78" t="s">
+        <v>63</v>
+      </c>
+      <c r="G45" s="79"/>
+      <c r="H45" s="80"/>
     </row>
     <row r="46" spans="2:8" ht="25.5">
       <c r="B46" s="20"/>
       <c r="C46" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D46" s="16">
         <v>41812</v>
       </c>
       <c r="E46" s="71" t="s">
-        <v>62</v>
-      </c>
-      <c r="F46" s="78" t="s">
-        <v>68</v>
-      </c>
-      <c r="G46" s="79"/>
-      <c r="H46" s="80"/>
+        <v>61</v>
+      </c>
+      <c r="F46" s="83" t="s">
+        <v>67</v>
+      </c>
+      <c r="G46" s="106"/>
+      <c r="H46" s="107"/>
     </row>
     <row r="47" spans="2:8" ht="14.25">
       <c r="B47" s="20"/>
       <c r="C47" s="68"/>
       <c r="D47" s="67"/>
       <c r="E47" s="67"/>
-      <c r="F47" s="81"/>
-      <c r="G47" s="82"/>
-      <c r="H47" s="83"/>
+      <c r="F47" s="78"/>
+      <c r="G47" s="79"/>
+      <c r="H47" s="80"/>
     </row>
     <row r="48" spans="2:8" ht="14.25">
       <c r="B48" s="20"/>
       <c r="C48" s="21"/>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
-      <c r="F48" s="78"/>
-      <c r="G48" s="79"/>
-      <c r="H48" s="80"/>
+      <c r="F48" s="83"/>
+      <c r="G48" s="106"/>
+      <c r="H48" s="107"/>
     </row>
     <row r="49" spans="2:8" ht="14.25">
       <c r="B49" s="20"/>
       <c r="C49" s="68"/>
       <c r="D49" s="67"/>
       <c r="E49" s="67"/>
-      <c r="F49" s="81"/>
-      <c r="G49" s="82"/>
-      <c r="H49" s="83"/>
+      <c r="F49" s="78"/>
+      <c r="G49" s="79"/>
+      <c r="H49" s="80"/>
     </row>
     <row r="50" spans="2:8" ht="14.25">
       <c r="B50" s="20"/>
       <c r="C50" s="22"/>
       <c r="D50" s="18"/>
       <c r="E50" s="18"/>
-      <c r="F50" s="84"/>
-      <c r="G50" s="85"/>
-      <c r="H50" s="86"/>
+      <c r="F50" s="98"/>
+      <c r="G50" s="99"/>
+      <c r="H50" s="100"/>
     </row>
     <row r="52" spans="2:8">
       <c r="B52" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D52" s="26" t="s">
         <v>7</v>
@@ -3986,11 +3987,11 @@
       <c r="E52" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F52" s="87" t="s">
+      <c r="F52" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="G52" s="88"/>
-      <c r="H52" s="89"/>
+      <c r="G52" s="102"/>
+      <c r="H52" s="103"/>
     </row>
     <row r="53" spans="2:8" ht="14.25">
       <c r="B53" s="19"/>
@@ -4003,11 +4004,11 @@
       <c r="E53" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F53" s="90" t="s">
-        <v>61</v>
-      </c>
-      <c r="G53" s="91"/>
-      <c r="H53" s="92"/>
+      <c r="F53" s="95" t="s">
+        <v>60</v>
+      </c>
+      <c r="G53" s="104"/>
+      <c r="H53" s="105"/>
     </row>
     <row r="54" spans="2:8" ht="14.25">
       <c r="B54" s="20"/>
@@ -4018,121 +4019,121 @@
         <v>41784</v>
       </c>
       <c r="E54" s="67" t="s">
-        <v>70</v>
-      </c>
-      <c r="F54" s="81" t="s">
-        <v>63</v>
-      </c>
-      <c r="G54" s="82"/>
-      <c r="H54" s="83"/>
+        <v>69</v>
+      </c>
+      <c r="F54" s="78" t="s">
+        <v>62</v>
+      </c>
+      <c r="G54" s="79"/>
+      <c r="H54" s="80"/>
     </row>
     <row r="55" spans="2:8" ht="25.5">
       <c r="B55" s="20"/>
       <c r="C55" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D55" s="16">
         <v>41786</v>
       </c>
       <c r="E55" s="71" t="s">
-        <v>70</v>
-      </c>
-      <c r="F55" s="78"/>
-      <c r="G55" s="79"/>
-      <c r="H55" s="80"/>
+        <v>69</v>
+      </c>
+      <c r="F55" s="83"/>
+      <c r="G55" s="106"/>
+      <c r="H55" s="107"/>
     </row>
     <row r="56" spans="2:8" ht="25.5">
       <c r="B56" s="20"/>
       <c r="C56" s="68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D56" s="67">
         <v>41791</v>
       </c>
       <c r="E56" s="67" t="s">
-        <v>70</v>
-      </c>
-      <c r="F56" s="81" t="s">
-        <v>64</v>
-      </c>
-      <c r="G56" s="82"/>
-      <c r="H56" s="83"/>
+        <v>69</v>
+      </c>
+      <c r="F56" s="78" t="s">
+        <v>63</v>
+      </c>
+      <c r="G56" s="79"/>
+      <c r="H56" s="80"/>
     </row>
     <row r="57" spans="2:8" ht="38.25">
       <c r="B57" s="20"/>
       <c r="C57" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D57" s="16">
         <v>41805</v>
       </c>
       <c r="E57" s="66" t="s">
-        <v>75</v>
-      </c>
-      <c r="F57" s="78" t="s">
-        <v>68</v>
-      </c>
-      <c r="G57" s="79"/>
-      <c r="H57" s="80"/>
+        <v>74</v>
+      </c>
+      <c r="F57" s="83" t="s">
+        <v>67</v>
+      </c>
+      <c r="G57" s="106"/>
+      <c r="H57" s="107"/>
     </row>
     <row r="58" spans="2:8" ht="38.25">
       <c r="B58" s="20"/>
       <c r="C58" s="68" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D58" s="67">
         <v>41812</v>
       </c>
       <c r="E58" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="F58" s="78" t="s">
         <v>75</v>
       </c>
-      <c r="F58" s="81" t="s">
-        <v>76</v>
-      </c>
-      <c r="G58" s="82"/>
-      <c r="H58" s="83"/>
+      <c r="G58" s="79"/>
+      <c r="H58" s="80"/>
     </row>
     <row r="59" spans="2:8" ht="25.5">
       <c r="B59" s="20"/>
       <c r="C59" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D59" s="16">
         <v>41812</v>
       </c>
       <c r="E59" s="74" t="s">
-        <v>77</v>
-      </c>
-      <c r="F59" s="78" t="s">
-        <v>79</v>
-      </c>
-      <c r="G59" s="79"/>
-      <c r="H59" s="80"/>
+        <v>76</v>
+      </c>
+      <c r="F59" s="83" t="s">
+        <v>78</v>
+      </c>
+      <c r="G59" s="106"/>
+      <c r="H59" s="107"/>
     </row>
     <row r="60" spans="2:8" ht="14.25">
       <c r="B60" s="20"/>
       <c r="C60" s="68"/>
       <c r="D60" s="67"/>
       <c r="E60" s="67"/>
-      <c r="F60" s="81"/>
-      <c r="G60" s="82"/>
-      <c r="H60" s="83"/>
+      <c r="F60" s="78"/>
+      <c r="G60" s="79"/>
+      <c r="H60" s="80"/>
     </row>
     <row r="61" spans="2:8" ht="14.25">
       <c r="B61" s="20"/>
       <c r="C61" s="22"/>
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
-      <c r="F61" s="84"/>
-      <c r="G61" s="85"/>
-      <c r="H61" s="86"/>
+      <c r="F61" s="98"/>
+      <c r="G61" s="99"/>
+      <c r="H61" s="100"/>
     </row>
     <row r="63" spans="2:8">
       <c r="B63" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C63" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D63" s="26" t="s">
         <v>7</v>
@@ -4140,16 +4141,16 @@
       <c r="E63" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F63" s="87" t="s">
+      <c r="F63" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="G63" s="88"/>
-      <c r="H63" s="89"/>
+      <c r="G63" s="102"/>
+      <c r="H63" s="103"/>
     </row>
     <row r="64" spans="2:8" ht="38.25">
       <c r="B64" s="19"/>
       <c r="C64" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D64" s="15">
         <v>41791</v>
@@ -4157,16 +4158,16 @@
       <c r="E64" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F64" s="90" t="s">
-        <v>82</v>
-      </c>
-      <c r="G64" s="91"/>
-      <c r="H64" s="92"/>
+      <c r="F64" s="95" t="s">
+        <v>81</v>
+      </c>
+      <c r="G64" s="104"/>
+      <c r="H64" s="105"/>
     </row>
     <row r="65" spans="2:8" ht="25.5">
       <c r="B65" s="20"/>
       <c r="C65" s="68" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D65" s="67">
         <v>41802</v>
@@ -4174,76 +4175,123 @@
       <c r="E65" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="F65" s="81"/>
-      <c r="G65" s="82"/>
-      <c r="H65" s="83"/>
+      <c r="F65" s="78"/>
+      <c r="G65" s="79"/>
+      <c r="H65" s="80"/>
     </row>
     <row r="66" spans="2:8" ht="14.25">
       <c r="B66" s="20"/>
       <c r="C66" s="21"/>
       <c r="D66" s="16"/>
       <c r="E66" s="71"/>
-      <c r="F66" s="78"/>
-      <c r="G66" s="79"/>
-      <c r="H66" s="80"/>
+      <c r="F66" s="83"/>
+      <c r="G66" s="106"/>
+      <c r="H66" s="107"/>
     </row>
     <row r="67" spans="2:8" ht="14.25">
       <c r="B67" s="20"/>
       <c r="C67" s="68"/>
       <c r="D67" s="67"/>
       <c r="E67" s="67"/>
-      <c r="F67" s="81"/>
-      <c r="G67" s="82"/>
-      <c r="H67" s="83"/>
+      <c r="F67" s="78"/>
+      <c r="G67" s="79"/>
+      <c r="H67" s="80"/>
     </row>
     <row r="68" spans="2:8" ht="14.25">
       <c r="B68" s="20"/>
       <c r="C68" s="21"/>
       <c r="D68" s="16"/>
       <c r="E68" s="66"/>
-      <c r="F68" s="78"/>
-      <c r="G68" s="79"/>
-      <c r="H68" s="80"/>
+      <c r="F68" s="83"/>
+      <c r="G68" s="106"/>
+      <c r="H68" s="107"/>
     </row>
     <row r="69" spans="2:8" ht="14.25">
       <c r="B69" s="20"/>
       <c r="C69" s="68"/>
       <c r="D69" s="67"/>
       <c r="E69" s="70"/>
-      <c r="F69" s="81"/>
-      <c r="G69" s="82"/>
-      <c r="H69" s="83"/>
+      <c r="F69" s="78"/>
+      <c r="G69" s="79"/>
+      <c r="H69" s="80"/>
     </row>
     <row r="70" spans="2:8" ht="14.25">
       <c r="B70" s="20"/>
       <c r="C70" s="21"/>
       <c r="D70" s="16"/>
       <c r="E70" s="74"/>
-      <c r="F70" s="78"/>
-      <c r="G70" s="79"/>
-      <c r="H70" s="80"/>
+      <c r="F70" s="83"/>
+      <c r="G70" s="106"/>
+      <c r="H70" s="107"/>
     </row>
     <row r="71" spans="2:8" ht="14.25">
       <c r="B71" s="20"/>
       <c r="C71" s="68"/>
       <c r="D71" s="67"/>
       <c r="E71" s="67"/>
-      <c r="F71" s="81"/>
-      <c r="G71" s="82"/>
-      <c r="H71" s="83"/>
+      <c r="F71" s="78"/>
+      <c r="G71" s="79"/>
+      <c r="H71" s="80"/>
     </row>
     <row r="72" spans="2:8" ht="14.25">
       <c r="B72" s="20"/>
       <c r="C72" s="22"/>
       <c r="D72" s="18"/>
       <c r="E72" s="18"/>
-      <c r="F72" s="84"/>
-      <c r="G72" s="85"/>
-      <c r="H72" s="86"/>
+      <c r="F72" s="98"/>
+      <c r="G72" s="99"/>
+      <c r="H72" s="100"/>
     </row>
   </sheetData>
   <autoFilter ref="B5:B38"/>
   <mergeCells count="60">
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F29:H29"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="F8:H8"/>
@@ -4257,53 +4305,6 @@
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="F72:H72"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>